<commit_message>
was dumb about red limits?
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -241,7 +241,7 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -317,124 +317,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>

</xml_diff>